<commit_message>
tam thoi xong man edit
</commit_message>
<xml_diff>
--- a/src/testdata/employeeManagementDta.xlsx
+++ b/src/testdata/employeeManagementDta.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="350">
   <si>
     <t>Description</t>
   </si>
@@ -1336,6 +1336,372 @@
   </si>
   <si>
     <t>nguyễn thị</t>
+  </si>
+  <si>
+    <t>OtherID</t>
+  </si>
+  <si>
+    <t>Driver_License_Number</t>
+  </si>
+  <si>
+    <t>Check value in dropdown and order value in dropdown
+Ex: Display full value equal DB</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Check when the date field is in an incorrect format.
+1. Enter a date value in an incorrect format:
+2. Check with the following formats: MM-DD-YYYY
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>04-05-2025</t>
+  </si>
+  <si>
+    <t>Should be a valid date in yyyy-mm-dd format</t>
+  </si>
+  <si>
+    <t>Check when the date field is in an incorrect format.
+1. Enter a date value in an incorrect format:
+2. Check with the following formats: YYYY-DD-MM
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>2025-20-12</t>
+  </si>
+  <si>
+    <t>Check when the date field is in an incorrect format.
+1. Enter a date value in an incorrect format:
+2. Check with the following formats: abcdefgh
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>Check when the date field is in an incorrect format.
+1. Enter a date value in an incorrect format:
+2. Check with the following formats: DD; e.g., 25
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Check when the date field is in an incorrect format.
+1. Enter a date value in an incorrect format:
+2. Check with the following formats: DD-MM; e.g., 25-12.
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>23-04</t>
+  </si>
+  <si>
+    <t>Check when the date field is in the YYYY-MM-DD format but is invalid.
+1. Enter the following values into the date field:
+Invalid day DD (out of range [1,31]); e.g., 2009-04-32.
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>2009-04-32</t>
+  </si>
+  <si>
+    <t>Check when the date field is in the YYYY-MM-DD format but is invalid.
+1. Enter the following values into the date field:
+Invalid month MM (out of range [1,12]); e.g., 2009-04-12.
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>2009-14-12</t>
+  </si>
+  <si>
+    <t>Check when the date field is in the YYYY-MM-DD format but is invalid.
+1. Enter the following values into the date field:
+Check with the following boundary values: 1983-04-31
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>1983-04-31</t>
+  </si>
+  <si>
+    <t>Check when the date field is in the YYYY-MM-DD format but is invalid.
+1. Enter the following values into the date field:
+Check with the following boundary values: 1983-06-31
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>1983-06-31</t>
+  </si>
+  <si>
+    <t>Check when the date field is in the YYYY-MM-DD format but is invalid.
+1. Enter the following values into the date field:
+Check with the following boundary values: 1983-09-31
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>1983-09-31</t>
+  </si>
+  <si>
+    <t>Check when the date field is in the YYYY-MM-DD format but is invalid.
+1. Enter the following values into the date field:
+Check with the following boundary values: 1983-11-31
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>1983-11-31</t>
+  </si>
+  <si>
+    <t>Check when the date field is in the YYYY-MM-DD format but is invalid.
+1. Enter the following values into the date field:
+Check with the following boundary values: 1983-02-30
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>1983-02-29</t>
+  </si>
+  <si>
+    <t>Check when the date field is in the YYYY-MM-DD format but is invalid.
+1. Enter the following values into the date field:
+Check with the following boundary values: 1983-02-29
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>Check when the date field is in the YYYY-MM-DD format but is invalid.
+1. Enter the following values into the date field: YYYY &lt; 1000 or YYYY &gt; 9999: 0999-02-01
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>0999-02-01</t>
+  </si>
+  <si>
+    <t>Check when the date field is in the YYYY-MM-DD format but is invalid.
+1. Enter the following values into the date field: YYYY &lt; 1000 or YYYY &gt; 9999: 99999-02-01
+Expected result:Display the error message "Should be a valid date in yyyy-mm-dd format"</t>
+  </si>
+  <si>
+    <t>99999-02-01</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 31 in months (1, 3, 5, 7, 8, 10, 12)
+1.Enter 2025-01-31 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-01-31</t>
+  </si>
+  <si>
+    <t>Check DB 
+3. Click Save
+Ex. Save successful</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 31 in months (1, 3, 5, 7, 8, 10, 12)
+1.Enter 2025-03-31 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-03-31</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 31 in months (1, 3, 5, 7, 8, 10, 12)
+1.Enter 2025-05-31 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-05-31</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 31 in months (1, 3, 5, 7, 8, 10, 12)
+1.Enter 2025-07-31 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-07-31</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 31 in months (1, 3, 5, 7, 8, 10, 12)
+1.Enter 2025-08-31 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-08-31</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 31 in months (1, 3, 5, 7, 8, 10, 12)
+1.Enter 2025-10-31 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-10-31</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 31 in months (1, 3, 5, 7, 8, 10, 12)
+1.Enter 2025-12-31 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-12-31</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+1980-02-29
+1.Enter 1980-02-29 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>1980-02-29</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+1983-02-28
+1.Enter 1983-02-28 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>1983-02-28</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 30 in months (4, 6, 9, 11)
+1.Enter 2025-04-30 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-04-30</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 30 in months (4, 6, 9, 11)
+1.Enter 2025-06-30 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-06-30</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 30 in months (4, 6, 9, 11)
+1.Enter 2025-09-30 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-09-30</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+Day 30 in months (4, 6, 9, 11)
+1.Enter 2025-11-30 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>2025-11-30</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+1983-10-10
+1.Enter 1983-10-10 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>1983-10-10</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+1000-02-01
+1.Enter 1000-02-01 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>1000-02-01</t>
+  </si>
+  <si>
+    <t>Check when the date field has a valid YYYY-MM-DD format.
+Check with the following values:
+9999-02-01
+1.Enter 9999-02-01 into the textbox.
+Expected: The entered value is displayed correctly.</t>
+  </si>
+  <si>
+    <t>9999-02-01</t>
+  </si>
+  <si>
+    <t>Check the functionality of the Calendar box.
+1. Click the Calendar icon next to the textbox.
+2. Select a date value from the Calendar box.
+Expected Result: The Calendar box closes after a date is selected.</t>
+  </si>
+  <si>
+    <t>Check the functionality of the Close button
+1.Click the Calendar icon next to the textbox.
+2. Click the Close button.
+Expected Result: The Calendar box closes immediately after the Close button is clicked.</t>
+  </si>
+  <si>
+    <t>Check the functionality of the Today button
+1. Click the Calendar icon next to the textbox.
+2. Click the Today button.
+Expected Result: The value in the Calendar is set to today’s date.</t>
+  </si>
+  <si>
+    <t>Check the functionality of the Clear button
+1. Click the Calendar icon next to the textbox.
+2. Select a date from the Calendar box.
+3. Click the Clear button.
+Expected Result: The value in the Calendar is cleared.</t>
+  </si>
+  <si>
+    <t>Check the focus in the Calendar box when the textbox does not contain data.
+1. Click the Calendar icon next to the textbox.
+2. Check the focused value in the Calendar box.
+Expected Result: The focus in the Calendar is on today’s date.</t>
+  </si>
+  <si>
+    <t>rgb(255, 123, 29)</t>
+  </si>
+  <si>
+    <t>Check the focus in the Calendar box when the textbox already contains data.
+Assume the date field already has a value (e.g., 2025-08-27):
+1. Click the Calendar icon next to the textbox.
+2. Check the focused value in the Calendar box.
+Expected Result: The focus in the Calendar is on the date that is already entered in the textbox.</t>
+  </si>
+  <si>
+    <t>2025-08-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender Radio </t>
+  </si>
+  <si>
+    <t>Verify Check radio button
+Ex: Check radio button successfully</t>
+  </si>
+  <si>
+    <t>Verify Uncheck radio button
+Ex: Uncheck radio button successfully</t>
   </si>
 </sst>
 </file>
@@ -2067,7 +2433,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2270,6 +2636,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
@@ -2808,10 +3195,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M228"/>
+  <dimension ref="A1:M336"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="60" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="E221" sqref="E221"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="60" topLeftCell="A332" workbookViewId="0">
+      <selection activeCell="A340" sqref="A340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5"/>
@@ -3996,7 +4383,7 @@
       <c r="J45" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="K45" s="68" t="s">
+      <c r="K45" s="75" t="s">
         <v>154</v>
       </c>
       <c r="L45" s="11"/>
@@ -7088,6 +7475,1485 @@
       </c>
       <c r="D228" s="67"/>
       <c r="E228" s="11"/>
+    </row>
+    <row r="229" customFormat="1" spans="1:5">
+      <c r="A229" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B229" s="66"/>
+      <c r="C229" s="66"/>
+      <c r="D229" s="66"/>
+      <c r="E229" s="9"/>
+    </row>
+    <row r="230" customFormat="1" ht="101.5" spans="1:5">
+      <c r="A230" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B230" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="C230" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D230" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="E230" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="231" customFormat="1" spans="1:5">
+      <c r="A231" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B231" s="67"/>
+      <c r="C231" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D231" s="67"/>
+      <c r="E231" s="11"/>
+    </row>
+    <row r="232" customFormat="1" ht="87" spans="1:5">
+      <c r="A232" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B232" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="C232" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D232" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="E232" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="233" customFormat="1" spans="1:5">
+      <c r="A233" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B233" s="67"/>
+      <c r="C233" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D233" s="67"/>
+      <c r="E233" s="11"/>
+    </row>
+    <row r="234" customFormat="1" ht="87" spans="1:5">
+      <c r="A234" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B234" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="C234" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D234" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="E234" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="235" customFormat="1" spans="1:5">
+      <c r="A235" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B235" s="67"/>
+      <c r="C235" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D235" s="67"/>
+      <c r="E235" s="11"/>
+    </row>
+    <row r="236" customFormat="1" ht="116" spans="1:5">
+      <c r="A236" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B236" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="C236" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D236" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="E236" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="237" customFormat="1" spans="1:5">
+      <c r="A237" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B237" s="67"/>
+      <c r="C237" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D237" s="67"/>
+      <c r="E237" s="11"/>
+    </row>
+    <row r="238" customFormat="1" ht="87" spans="1:5">
+      <c r="A238" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B238" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C238" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D238" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="E238" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="239" customFormat="1" spans="1:5">
+      <c r="A239" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B239" s="67"/>
+      <c r="C239" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D239" s="67"/>
+      <c r="E239" s="11"/>
+    </row>
+    <row r="240" customFormat="1" ht="87" spans="1:5">
+      <c r="A240" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B240" s="67" t="s">
+        <v>156</v>
+      </c>
+      <c r="C240" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D240" s="67" t="s">
+        <v>156</v>
+      </c>
+      <c r="E240" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="241" customFormat="1" spans="1:5">
+      <c r="A241" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B241" s="67"/>
+      <c r="C241" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D241" s="67"/>
+      <c r="E241" s="11"/>
+    </row>
+    <row r="242" customFormat="1" ht="130.5" spans="1:5">
+      <c r="A242" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B242" s="67" t="s">
+        <v>162</v>
+      </c>
+      <c r="C242" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D242" s="67" t="s">
+        <v>162</v>
+      </c>
+      <c r="E242" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="243" customFormat="1" spans="1:5">
+      <c r="A243" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B243" s="67"/>
+      <c r="C243" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D243" s="67"/>
+      <c r="E243" s="11"/>
+    </row>
+    <row r="244" customFormat="1" ht="101.5" spans="1:5">
+      <c r="A244" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B244" s="67" t="s">
+        <v>271</v>
+      </c>
+      <c r="C244" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D244" s="67" t="s">
+        <v>271</v>
+      </c>
+      <c r="E244" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="245" customFormat="1" spans="1:5">
+      <c r="A245" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B245" s="67"/>
+      <c r="C245" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D245" s="67"/>
+      <c r="E245" s="11"/>
+    </row>
+    <row r="246" customFormat="1" spans="1:5">
+      <c r="A246" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B246" s="66"/>
+      <c r="C246" s="66"/>
+      <c r="D246" s="66"/>
+      <c r="E246" s="9"/>
+    </row>
+    <row r="247" customFormat="1" ht="101.5" spans="1:5">
+      <c r="A247" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B247" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="C247" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D247" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="E247" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="248" customFormat="1" spans="1:5">
+      <c r="A248" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B248" s="67"/>
+      <c r="C248" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D248" s="67"/>
+      <c r="E248" s="11"/>
+    </row>
+    <row r="249" customFormat="1" ht="87" spans="1:5">
+      <c r="A249" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B249" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="C249" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D249" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="E249" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="250" customFormat="1" spans="1:5">
+      <c r="A250" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B250" s="67"/>
+      <c r="C250" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D250" s="67"/>
+      <c r="E250" s="11"/>
+    </row>
+    <row r="251" customFormat="1" ht="87" spans="1:5">
+      <c r="A251" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B251" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="C251" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D251" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="E251" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="252" customFormat="1" spans="1:5">
+      <c r="A252" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B252" s="67"/>
+      <c r="C252" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D252" s="67"/>
+      <c r="E252" s="11"/>
+    </row>
+    <row r="253" customFormat="1" ht="116" spans="1:5">
+      <c r="A253" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B253" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="C253" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D253" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="E253" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="254" customFormat="1" spans="1:5">
+      <c r="A254" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B254" s="67"/>
+      <c r="C254" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D254" s="67"/>
+      <c r="E254" s="11"/>
+    </row>
+    <row r="255" customFormat="1" ht="87" spans="1:5">
+      <c r="A255" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B255" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C255" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D255" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="E255" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="256" customFormat="1" spans="1:5">
+      <c r="A256" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B256" s="67"/>
+      <c r="C256" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D256" s="67"/>
+      <c r="E256" s="11"/>
+    </row>
+    <row r="257" customFormat="1" ht="87" spans="1:5">
+      <c r="A257" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B257" s="67" t="s">
+        <v>156</v>
+      </c>
+      <c r="C257" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D257" s="67" t="s">
+        <v>156</v>
+      </c>
+      <c r="E257" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="258" customFormat="1" spans="1:5">
+      <c r="A258" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B258" s="67"/>
+      <c r="C258" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D258" s="67"/>
+      <c r="E258" s="11"/>
+    </row>
+    <row r="259" customFormat="1" ht="130.5" spans="1:5">
+      <c r="A259" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B259" s="67" t="s">
+        <v>162</v>
+      </c>
+      <c r="C259" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D259" s="67" t="s">
+        <v>162</v>
+      </c>
+      <c r="E259" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="260" customFormat="1" spans="1:5">
+      <c r="A260" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B260" s="67"/>
+      <c r="C260" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D260" s="67"/>
+      <c r="E260" s="11"/>
+    </row>
+    <row r="261" customFormat="1" ht="101.5" spans="1:5">
+      <c r="A261" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B261" s="67" t="s">
+        <v>271</v>
+      </c>
+      <c r="C261" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D261" s="67" t="s">
+        <v>271</v>
+      </c>
+      <c r="E261" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="262" customFormat="1" spans="1:5">
+      <c r="A262" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B262" s="67"/>
+      <c r="C262" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D262" s="67"/>
+      <c r="E262" s="11"/>
+    </row>
+    <row r="263" spans="1:5">
+      <c r="A263" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B263" s="62"/>
+      <c r="C263" s="62"/>
+      <c r="D263" s="62"/>
+      <c r="E263" s="62"/>
+    </row>
+    <row r="264" ht="29" spans="1:6">
+      <c r="A264" s="63" t="s">
+        <v>274</v>
+      </c>
+      <c r="B264" s="24"/>
+      <c r="C264" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="D264" s="24"/>
+      <c r="E264" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F264" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="265" s="2" customFormat="1" spans="1:5">
+      <c r="A265" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B265" s="66"/>
+      <c r="C265" s="66"/>
+      <c r="D265" s="66"/>
+      <c r="E265" s="9"/>
+    </row>
+    <row r="266" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A266" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B266" s="67" t="s">
+        <v>278</v>
+      </c>
+      <c r="C266" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D266" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E266" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="267" s="2" customFormat="1" spans="1:5">
+      <c r="A267" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B267" s="67"/>
+      <c r="C267" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D267" s="67"/>
+      <c r="E267" s="11"/>
+    </row>
+    <row r="268" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A268" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B268" s="67" t="s">
+        <v>281</v>
+      </c>
+      <c r="C268" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D268" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E268" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="269" s="2" customFormat="1" spans="1:5">
+      <c r="A269" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B269" s="67"/>
+      <c r="C269" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D269" s="67"/>
+      <c r="E269" s="11"/>
+    </row>
+    <row r="270" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A270" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B270" s="67" t="s">
+        <v>212</v>
+      </c>
+      <c r="C270" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D270" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E270" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="271" s="2" customFormat="1" spans="1:5">
+      <c r="A271" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B271" s="67"/>
+      <c r="C271" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D271" s="67"/>
+      <c r="E271" s="11"/>
+    </row>
+    <row r="272" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A272" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B272" s="67" t="s">
+        <v>284</v>
+      </c>
+      <c r="C272" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D272" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E272" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="273" s="2" customFormat="1" spans="1:5">
+      <c r="A273" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B273" s="67"/>
+      <c r="C273" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D273" s="67"/>
+      <c r="E273" s="11"/>
+    </row>
+    <row r="274" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A274" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="B274" s="67" t="s">
+        <v>286</v>
+      </c>
+      <c r="C274" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D274" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E274" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="275" s="2" customFormat="1" spans="1:5">
+      <c r="A275" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B275" s="67"/>
+      <c r="C275" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D275" s="67"/>
+      <c r="E275" s="11"/>
+    </row>
+    <row r="276" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A276" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="B276" s="67" t="s">
+        <v>288</v>
+      </c>
+      <c r="C276" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D276" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E276" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="277" s="2" customFormat="1" spans="1:5">
+      <c r="A277" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B277" s="67"/>
+      <c r="C277" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D277" s="67"/>
+      <c r="E277" s="11"/>
+    </row>
+    <row r="278" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A278" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B278" s="67" t="s">
+        <v>290</v>
+      </c>
+      <c r="C278" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D278" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E278" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="279" s="2" customFormat="1" spans="1:5">
+      <c r="A279" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B279" s="67"/>
+      <c r="C279" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D279" s="67"/>
+      <c r="E279" s="11"/>
+    </row>
+    <row r="280" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A280" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="B280" s="67" t="s">
+        <v>292</v>
+      </c>
+      <c r="C280" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D280" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E280" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="281" s="2" customFormat="1" spans="1:5">
+      <c r="A281" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B281" s="67"/>
+      <c r="C281" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D281" s="67"/>
+      <c r="E281" s="11"/>
+    </row>
+    <row r="282" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A282" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B282" s="67" t="s">
+        <v>294</v>
+      </c>
+      <c r="C282" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D282" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E282" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="283" s="2" customFormat="1" spans="1:5">
+      <c r="A283" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B283" s="67"/>
+      <c r="C283" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D283" s="67"/>
+      <c r="E283" s="11"/>
+    </row>
+    <row r="284" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A284" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B284" s="67" t="s">
+        <v>296</v>
+      </c>
+      <c r="C284" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D284" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E284" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="285" s="2" customFormat="1" spans="1:5">
+      <c r="A285" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B285" s="67"/>
+      <c r="C285" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D285" s="67"/>
+      <c r="E285" s="11"/>
+    </row>
+    <row r="286" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A286" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B286" s="67" t="s">
+        <v>298</v>
+      </c>
+      <c r="C286" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D286" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E286" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="287" s="2" customFormat="1" spans="1:5">
+      <c r="A287" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B287" s="67"/>
+      <c r="C287" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D287" s="67"/>
+      <c r="E287" s="11"/>
+    </row>
+    <row r="288" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A288" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="B288" s="67" t="s">
+        <v>300</v>
+      </c>
+      <c r="C288" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D288" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E288" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="289" s="2" customFormat="1" spans="1:5">
+      <c r="A289" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B289" s="67"/>
+      <c r="C289" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D289" s="67"/>
+      <c r="E289" s="11"/>
+    </row>
+    <row r="290" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A290" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B290" s="67" t="s">
+        <v>300</v>
+      </c>
+      <c r="C290" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D290" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E290" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="291" s="2" customFormat="1" spans="1:5">
+      <c r="A291" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B291" s="67"/>
+      <c r="C291" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D291" s="67"/>
+      <c r="E291" s="11"/>
+    </row>
+    <row r="292" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A292" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B292" s="67" t="s">
+        <v>303</v>
+      </c>
+      <c r="C292" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D292" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E292" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="293" s="2" customFormat="1" spans="1:5">
+      <c r="A293" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B293" s="67"/>
+      <c r="C293" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D293" s="67"/>
+      <c r="E293" s="11"/>
+    </row>
+    <row r="294" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A294" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B294" s="67" t="s">
+        <v>305</v>
+      </c>
+      <c r="C294" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D294" s="67" t="s">
+        <v>279</v>
+      </c>
+      <c r="E294" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="295" s="2" customFormat="1" spans="1:5">
+      <c r="A295" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B295" s="67"/>
+      <c r="C295" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D295" s="67"/>
+      <c r="E295" s="11"/>
+    </row>
+    <row r="296" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A296" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="B296" s="67" t="s">
+        <v>307</v>
+      </c>
+      <c r="C296" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D296" s="67" t="s">
+        <v>307</v>
+      </c>
+      <c r="E296" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="297" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A297" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B297" s="67"/>
+      <c r="C297" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D297" s="67"/>
+      <c r="E297" s="11"/>
+    </row>
+    <row r="298" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A298" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="B298" s="67" t="s">
+        <v>310</v>
+      </c>
+      <c r="C298" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D298" s="67" t="s">
+        <v>310</v>
+      </c>
+      <c r="E298" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="299" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A299" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B299" s="67"/>
+      <c r="C299" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D299" s="67"/>
+      <c r="E299" s="11"/>
+    </row>
+    <row r="300" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A300" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="B300" s="67" t="s">
+        <v>312</v>
+      </c>
+      <c r="C300" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D300" s="67" t="s">
+        <v>312</v>
+      </c>
+      <c r="E300" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="301" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A301" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B301" s="67"/>
+      <c r="C301" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D301" s="67"/>
+      <c r="E301" s="11"/>
+    </row>
+    <row r="302" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A302" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="B302" s="67" t="s">
+        <v>314</v>
+      </c>
+      <c r="C302" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D302" s="67" t="s">
+        <v>314</v>
+      </c>
+      <c r="E302" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="303" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A303" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B303" s="67"/>
+      <c r="C303" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D303" s="67"/>
+      <c r="E303" s="11"/>
+    </row>
+    <row r="304" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A304" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="B304" s="67" t="s">
+        <v>316</v>
+      </c>
+      <c r="C304" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D304" s="67" t="s">
+        <v>316</v>
+      </c>
+      <c r="E304" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="305" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A305" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B305" s="67"/>
+      <c r="C305" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D305" s="67"/>
+      <c r="E305" s="11"/>
+    </row>
+    <row r="306" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A306" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B306" s="67" t="s">
+        <v>318</v>
+      </c>
+      <c r="C306" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D306" s="67" t="s">
+        <v>318</v>
+      </c>
+      <c r="E306" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="307" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A307" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B307" s="67"/>
+      <c r="C307" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D307" s="67"/>
+      <c r="E307" s="11"/>
+    </row>
+    <row r="308" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A308" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="B308" s="67" t="s">
+        <v>320</v>
+      </c>
+      <c r="C308" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D308" s="67" t="s">
+        <v>320</v>
+      </c>
+      <c r="E308" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="309" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A309" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B309" s="67"/>
+      <c r="C309" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D309" s="67"/>
+      <c r="E309" s="11"/>
+    </row>
+    <row r="310" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A310" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="B310" s="67" t="s">
+        <v>322</v>
+      </c>
+      <c r="C310" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D310" s="67" t="s">
+        <v>322</v>
+      </c>
+      <c r="E310" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="311" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A311" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B311" s="67"/>
+      <c r="C311" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D311" s="67"/>
+      <c r="E311" s="11"/>
+    </row>
+    <row r="312" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A312" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="B312" s="67" t="s">
+        <v>324</v>
+      </c>
+      <c r="C312" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D312" s="67" t="s">
+        <v>324</v>
+      </c>
+      <c r="E312" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="313" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A313" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B313" s="67"/>
+      <c r="C313" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D313" s="67"/>
+      <c r="E313" s="11"/>
+    </row>
+    <row r="314" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A314" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="B314" s="67" t="s">
+        <v>326</v>
+      </c>
+      <c r="C314" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D314" s="67" t="s">
+        <v>326</v>
+      </c>
+      <c r="E314" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="315" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A315" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B315" s="67"/>
+      <c r="C315" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D315" s="67"/>
+      <c r="E315" s="11"/>
+    </row>
+    <row r="316" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A316" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="B316" s="67" t="s">
+        <v>328</v>
+      </c>
+      <c r="C316" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D316" s="67" t="s">
+        <v>328</v>
+      </c>
+      <c r="E316" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="317" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A317" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B317" s="67"/>
+      <c r="C317" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D317" s="67"/>
+      <c r="E317" s="11"/>
+    </row>
+    <row r="318" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A318" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="B318" s="67" t="s">
+        <v>330</v>
+      </c>
+      <c r="C318" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D318" s="67" t="s">
+        <v>330</v>
+      </c>
+      <c r="E318" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="319" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A319" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B319" s="67"/>
+      <c r="C319" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D319" s="67"/>
+      <c r="E319" s="11"/>
+    </row>
+    <row r="320" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A320" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="B320" s="67" t="s">
+        <v>332</v>
+      </c>
+      <c r="C320" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D320" s="67" t="s">
+        <v>332</v>
+      </c>
+      <c r="E320" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="321" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A321" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B321" s="67"/>
+      <c r="C321" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D321" s="67"/>
+      <c r="E321" s="11"/>
+    </row>
+    <row r="322" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A322" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="B322" s="67" t="s">
+        <v>334</v>
+      </c>
+      <c r="C322" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D322" s="67" t="s">
+        <v>334</v>
+      </c>
+      <c r="E322" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="323" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A323" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B323" s="67"/>
+      <c r="C323" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D323" s="67"/>
+      <c r="E323" s="11"/>
+    </row>
+    <row r="324" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A324" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="B324" s="67" t="s">
+        <v>336</v>
+      </c>
+      <c r="C324" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D324" s="67" t="s">
+        <v>336</v>
+      </c>
+      <c r="E324" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="325" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A325" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B325" s="67"/>
+      <c r="C325" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D325" s="67"/>
+      <c r="E325" s="11"/>
+    </row>
+    <row r="326" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A326" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="B326" s="67" t="s">
+        <v>338</v>
+      </c>
+      <c r="C326" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="D326" s="67" t="s">
+        <v>338</v>
+      </c>
+      <c r="E326" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="327" s="2" customFormat="1" ht="43.5" spans="1:5">
+      <c r="A327" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B327" s="67"/>
+      <c r="C327" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D327" s="67"/>
+      <c r="E327" s="11"/>
+    </row>
+    <row r="328" s="2" customFormat="1" ht="58" spans="1:5">
+      <c r="A328" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="B328" s="11"/>
+      <c r="C328" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="D328" s="11"/>
+      <c r="E328" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="329" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A329" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B329" s="11"/>
+      <c r="C329" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="D329" s="11"/>
+      <c r="E329" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="330" s="2" customFormat="1" ht="58" spans="1:5">
+      <c r="A330" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="B330" s="68"/>
+      <c r="C330" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="D330" s="11"/>
+      <c r="E330" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="331" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A331" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="B331" s="68"/>
+      <c r="C331" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="D331" s="11"/>
+      <c r="E331" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="332" s="2" customFormat="1" ht="72.5" spans="1:5">
+      <c r="A332" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="B332" s="69"/>
+      <c r="C332" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="D332" s="67" t="s">
+        <v>344</v>
+      </c>
+      <c r="E332" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="333" s="2" customFormat="1" ht="101.5" spans="1:5">
+      <c r="A333" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="B333" s="70" t="s">
+        <v>346</v>
+      </c>
+      <c r="C333" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="D333" s="70" t="s">
+        <v>344</v>
+      </c>
+      <c r="E333" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5">
+      <c r="A334" s="71" t="s">
+        <v>347</v>
+      </c>
+      <c r="B334" s="72"/>
+      <c r="C334" s="72"/>
+      <c r="D334" s="72"/>
+      <c r="E334" s="72"/>
+    </row>
+    <row r="335" ht="29" spans="1:5">
+      <c r="A335" s="73" t="s">
+        <v>348</v>
+      </c>
+      <c r="B335" s="74"/>
+      <c r="C335" s="74"/>
+      <c r="D335" s="74"/>
+      <c r="E335" s="74"/>
+    </row>
+    <row r="336" ht="29" spans="1:5">
+      <c r="A336" s="73" t="s">
+        <v>349</v>
+      </c>
+      <c r="B336" s="74"/>
+      <c r="C336" s="74"/>
+      <c r="D336" s="74"/>
+      <c r="E336" s="74"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
tạm xong module timesheet
</commit_message>
<xml_diff>
--- a/src/testdata/employeeManagementDta.xlsx
+++ b/src/testdata/employeeManagementDta.xlsx
@@ -3197,8 +3197,8 @@
   <sheetPr/>
   <dimension ref="A1:M336"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="60" topLeftCell="A332" workbookViewId="0">
-      <selection activeCell="A340" sqref="A340"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="60" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5"/>

</xml_diff>